<commit_message>
change in main tzlil
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7360" windowWidth="14400" xWindow="380" yWindow="380"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -330,13 +317,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">correct </t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>not correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add func to add new line
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -404,6 +404,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
xlsx and unittest update
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -448,6 +448,105 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>